<commit_message>
Added automatic email generation
</commit_message>
<xml_diff>
--- a/assets/temp.xlsx
+++ b/assets/temp.xlsx
@@ -403,7 +403,7 @@
       </c>
       <c r="B1" s="11" t="inlineStr">
         <is>
-          <t>00061095</t>
+          <t>00061382</t>
         </is>
       </c>
       <c r="C1" s="3" t="n"/>
@@ -414,7 +414,7 @@
       </c>
       <c r="F1" s="11" t="inlineStr">
         <is>
-          <t>Trent Waters</t>
+          <t>Benjamin Munoz</t>
         </is>
       </c>
       <c r="G1" s="3" t="n"/>
@@ -435,7 +435,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>300006818</t>
+          <t>300006827</t>
         </is>
       </c>
       <c r="C3" s="3" t="n"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="F3" s="11" t="inlineStr">
         <is>
-          <t>Trent Waters</t>
+          <t>Benjamin Munoz</t>
         </is>
       </c>
       <c r="G3" s="3" t="n"/>
@@ -464,7 +464,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>0880011908</t>
+          <t>0880011926</t>
         </is>
       </c>
       <c r="C5" s="7" t="inlineStr">
@@ -479,7 +479,7 @@
       </c>
       <c r="F5" s="11" t="inlineStr">
         <is>
-          <t>01/23</t>
+          <t>01/24</t>
         </is>
       </c>
       <c r="G5" s="3" t="n"/>
@@ -511,7 +511,7 @@
       <c r="C10" s="6" t="n"/>
       <c r="E10" s="12" t="inlineStr">
         <is>
-          <t>drone crashed returning home. guy wrote an essay about it, check sf</t>
+          <t>customer said the craft shut down and fell 100 ft to the ground during the rth, he thought it was a product issue, not his responsibility, so asked for a data analysis</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed label bug, and fixed bug where sap would not reload manager on new form creation
</commit_message>
<xml_diff>
--- a/assets/temp.xlsx
+++ b/assets/temp.xlsx
@@ -403,7 +403,7 @@
       </c>
       <c r="B1" s="11" t="inlineStr">
         <is>
-          <t>00059171</t>
+          <t>00060992</t>
         </is>
       </c>
       <c r="C1" s="3" t="n"/>
@@ -414,7 +414,7 @@
       </c>
       <c r="F1" s="11" t="inlineStr">
         <is>
-          <t>Christopher Felski</t>
+          <t>Hector Venzor</t>
         </is>
       </c>
       <c r="G1" s="3" t="n"/>
@@ -435,7 +435,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>300006839</t>
+          <t>300006848</t>
         </is>
       </c>
       <c r="C3" s="3" t="n"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="F3" s="11" t="inlineStr">
         <is>
-          <t>Christopher Felski</t>
+          <t>Hector Venzor</t>
         </is>
       </c>
       <c r="G3" s="3" t="n"/>
@@ -464,7 +464,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>0880011949</t>
+          <t>0880011962</t>
         </is>
       </c>
       <c r="C5" s="7" t="inlineStr">
@@ -511,7 +511,7 @@
       <c r="C10" s="6" t="n"/>
       <c r="E10" s="12" t="inlineStr">
         <is>
-          <t>prop damage due to limb strike. props incorrectly replaced resulting in rollover crashes. this may have resulted in broken motor arm and gimble damage.</t>
+          <t>said safe to fly i swiped for it to fly went up and shot it self backwards into a fence propellers broke and crack on side of a leg on body</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed nonfunctional repair form
</commit_message>
<xml_diff>
--- a/assets/temp.xlsx
+++ b/assets/temp.xlsx
@@ -403,7 +403,7 @@
       </c>
       <c r="B1" s="11" t="inlineStr">
         <is>
-          <t>00070973</t>
+          <t>00069790</t>
         </is>
       </c>
       <c r="C1" s="3" t="n"/>
@@ -414,7 +414,7 @@
       </c>
       <c r="F1" s="11" t="inlineStr">
         <is>
-          <t>Tyler Davis</t>
+          <t>Sussie Due</t>
         </is>
       </c>
       <c r="G1" s="3" t="n"/>
@@ -435,7 +435,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>300007196</t>
+          <t>300007240</t>
         </is>
       </c>
       <c r="C3" s="3" t="n"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="F3" s="11" t="inlineStr">
         <is>
-          <t>Tyler Davis</t>
+          <t>Sussie Due</t>
         </is>
       </c>
       <c r="G3" s="3" t="n"/>
@@ -464,7 +464,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>0880012602</t>
+          <t>0880012712</t>
         </is>
       </c>
       <c r="C5" s="7" t="inlineStr">
@@ -479,7 +479,7 @@
       </c>
       <c r="F5" s="11" t="inlineStr">
         <is>
-          <t>04/15</t>
+          <t>04/23</t>
         </is>
       </c>
       <c r="G5" s="3" t="n"/>
@@ -509,7 +509,11 @@
       <c r="A10" s="4" t="n"/>
       <c r="B10" s="8" t="n"/>
       <c r="C10" s="6" t="n"/>
-      <c r="E10" s="12" t="inlineStr"/>
+      <c r="E10" s="12" t="inlineStr">
+        <is>
+          <t>upon determination, there is a problem as soon as the box is open. please provide warranty service.</t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="9">
       <c r="A11" s="1" t="inlineStr">

</xml_diff>